<commit_message>
fixing model equations and adding county column
</commit_message>
<xml_diff>
--- a/HsSurvey_glm_lm_model_fits.xlsx
+++ b/HsSurvey_glm_lm_model_fits.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Camille\Desktop\Fishscapes\hsSurvey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F95C19B-9939-4880-A04A-1677199223CD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7D7DC4B-7932-47A4-BC67-10D04022A383}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="449" activeTab="1" xr2:uid="{17A9F256-7631-491B-A39B-0452DB16D56A}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="43">
   <si>
     <t>&lt; 2e-16</t>
   </si>
@@ -156,6 +156,12 @@
   </si>
   <si>
     <t>bassbuildCWHJoin$logAbun:bassbuildCWHJoin$Total.CWH.per.km.shoreline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lake year CPUE county table for all observations </t>
+  </si>
+  <si>
+    <t xml:space="preserve">note proportions of Vilas and Oneida dominate </t>
   </si>
 </sst>
 </file>
@@ -365,6 +371,55 @@
         <a:xfrm>
           <a:off x="0" y="4191000"/>
           <a:ext cx="5000000" cy="3247619"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>18209</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>28452</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F403C418-2368-46A9-98A0-CDFA39158F2D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="7810500"/>
+          <a:ext cx="6723809" cy="980952"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -675,7 +730,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ED3D0C4-5DCE-41DD-8AD0-6E560E0C7C68}">
   <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
+    <sheetView topLeftCell="A61" workbookViewId="0">
       <selection activeCell="F57" sqref="F57"/>
     </sheetView>
   </sheetViews>
@@ -1442,14 +1497,101 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE8A2B24-0049-4E24-AA3F-F6D500EED1EB}">
-  <dimension ref="A1"/>
+  <dimension ref="A41:L46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="L41" sqref="L41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
+      <c r="J41" s="1"/>
+      <c r="K41" s="1"/>
+      <c r="L41" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42" s="2"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
+      <c r="I42" s="2"/>
+      <c r="J42" s="2"/>
+      <c r="K42" s="2"/>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43" s="2"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
+      <c r="J43" s="2"/>
+      <c r="K43" s="2"/>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A44" s="2"/>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
+      <c r="J44" s="2"/>
+      <c r="K44" s="2"/>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A45" s="2"/>
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2"/>
+      <c r="I45" s="2"/>
+      <c r="J45" s="2"/>
+      <c r="K45" s="2"/>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A46" s="2"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="2"/>
+      <c r="H46" s="2"/>
+      <c r="I46" s="2"/>
+      <c r="J46" s="2"/>
+      <c r="K46" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A41:K41"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>